<commit_message>
Update for Manuscript Submission
</commit_message>
<xml_diff>
--- a/Res_2_Results/Res_SummaryT_Subgroup_Dep.xlsx
+++ b/Res_2_Results/Res_SummaryT_Subgroup_Dep.xlsx
@@ -1,76 +1,68 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\ProfFang_Data\DataAnalysis\Res_2_Results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB25EC8-A34B-4867-BA81-C890A6D1D44A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="194">
-  <si>
-    <t>Index</t>
-  </si>
-  <si>
-    <t>Boy</t>
-  </si>
-  <si>
-    <t>Girl</t>
-  </si>
-  <si>
-    <t>Effect Size (Sex)</t>
-  </si>
-  <si>
-    <t>p-value (Sex)</t>
-  </si>
-  <si>
-    <t>PrimarySchool</t>
-  </si>
-  <si>
-    <t>JuniorSchool</t>
-  </si>
-  <si>
-    <t>SeniorSchool</t>
-  </si>
-  <si>
-    <t>Effect Size (Phase of studying)</t>
-  </si>
-  <si>
-    <t>p-value (Phase of studying)</t>
-  </si>
-  <si>
-    <t>Eastern</t>
-  </si>
-  <si>
-    <t>Northeast</t>
-  </si>
-  <si>
-    <t>Central</t>
-  </si>
-  <si>
-    <t>Western</t>
-  </si>
-  <si>
-    <t>Effect Size (Geographic Area)</t>
-  </si>
-  <si>
-    <t>p-value (Geographic Area)</t>
-  </si>
-  <si>
-    <t>ACC</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="181">
+  <si>
+    <t xml:space="preserve">Index</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Girl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Effect Size (Sex)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p-value (Sex)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PrimarySchool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JuniorSchool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SeniorSchool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Effect Size (Phase of studying)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p-value (Phase of studying)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eastern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northeast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Western</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Effect Size (Geographic Area)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p-value (Geographic Area)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACC</t>
   </si>
   <si>
     <t xml:space="preserve">83.69% (0.15%) </t>
@@ -79,10 +71,10 @@
     <t xml:space="preserve">86.27% (0.12%) </t>
   </si>
   <si>
-    <t>0.03 [0.03, 0.03]</t>
-  </si>
-  <si>
-    <t>&lt;0.001</t>
+    <t xml:space="preserve">0.03 [0.03, 0.03]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;0.001</t>
   </si>
   <si>
     <t xml:space="preserve">85.80% (0.21%) </t>
@@ -94,7 +86,7 @@
     <t xml:space="preserve">84.00% (0.16%) </t>
   </si>
   <si>
-    <t>.956 [.954, .958]</t>
+    <t xml:space="preserve">.956 [.954, .958]</t>
   </si>
   <si>
     <t xml:space="preserve">83.71% (0.14%) </t>
@@ -109,10 +101,10 @@
     <t xml:space="preserve">87.48% (0.17%) </t>
   </si>
   <si>
-    <t>.986 [.983, .986]</t>
-  </si>
-  <si>
-    <t>Sensitivity</t>
+    <t xml:space="preserve">.986 [.983, .986]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensitivity</t>
   </si>
   <si>
     <t xml:space="preserve">88.12% (0.18%) </t>
@@ -121,7 +113,7 @@
     <t xml:space="preserve">89.95% (0.15%) </t>
   </si>
   <si>
-    <t>0.02 [0.02, 0.02]</t>
+    <t xml:space="preserve">0.02 [0.02, 0.02]</t>
   </si>
   <si>
     <t xml:space="preserve">89.22% (0.24%) </t>
@@ -133,7 +125,7 @@
     <t xml:space="preserve">87.50% (0.20%) </t>
   </si>
   <si>
-    <t>.922 [.918, .925]</t>
+    <t xml:space="preserve">.922 [.918, .925]</t>
   </si>
   <si>
     <t xml:space="preserve">88.36% (0.21%) </t>
@@ -148,10 +140,10 @@
     <t xml:space="preserve">86.78% (0.25%) </t>
   </si>
   <si>
-    <t>.960 [.959, .965]</t>
-  </si>
-  <si>
-    <t>Specificity</t>
+    <t xml:space="preserve">.960 [.959, .965]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specificity</t>
   </si>
   <si>
     <t xml:space="preserve">83.36% (0.17%) </t>
@@ -169,7 +161,7 @@
     <t xml:space="preserve">83.56% (0.20%) </t>
   </si>
   <si>
-    <t>.953 [.951, .955]</t>
+    <t xml:space="preserve">.953 [.951, .955]</t>
   </si>
   <si>
     <t xml:space="preserve">83.37% (0.17%) </t>
@@ -184,10 +176,10 @@
     <t xml:space="preserve">87.54% (0.20%) </t>
   </si>
   <si>
-    <t>.985 [.983, .985]</t>
-  </si>
-  <si>
-    <t>Balanced ACC</t>
+    <t xml:space="preserve">.985 [.983, .985]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balanced ACC</t>
   </si>
   <si>
     <t xml:space="preserve">85.74% (0.02%) </t>
@@ -205,7 +197,7 @@
     <t xml:space="preserve">85.53% (0.02%) </t>
   </si>
   <si>
-    <t>.998 [.998, .998]</t>
+    <t xml:space="preserve">.998 [.998, .998]</t>
   </si>
   <si>
     <t xml:space="preserve">85.86% (0.04%) </t>
@@ -220,10 +212,10 @@
     <t xml:space="preserve">87.16% (0.04%) </t>
   </si>
   <si>
-    <t>.992 [.992, .993]</t>
-  </si>
-  <si>
-    <t>F1-score</t>
+    <t xml:space="preserve">.992 [.992, .993]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1-score</t>
   </si>
   <si>
     <t xml:space="preserve">0.4268 (0.0017) </t>
@@ -232,7 +224,7 @@
     <t xml:space="preserve">0.5265 (0.0018) </t>
   </si>
   <si>
-    <t>0.10 [0.10, 0.10]</t>
+    <t xml:space="preserve">0.10 [0.10, 0.10]</t>
   </si>
   <si>
     <t xml:space="preserve">0.3543 (0.0029) </t>
@@ -244,7 +236,7 @@
     <t xml:space="preserve">0.5479 (0.0019) </t>
   </si>
   <si>
-    <t>.999 [.999, .999]</t>
+    <t xml:space="preserve">.999 [.999, .999]</t>
   </si>
   <si>
     <t xml:space="preserve">0.4227 (0.0016) </t>
@@ -259,10 +251,10 @@
     <t xml:space="preserve">0.5215 (0.0026) </t>
   </si>
   <si>
-    <t>.994 [.994, .995]</t>
-  </si>
-  <si>
-    <t>PPV</t>
+    <t xml:space="preserve">.994 [.994, .995]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPV</t>
   </si>
   <si>
     <t xml:space="preserve">28.16% (0.17%) </t>
@@ -271,7 +263,7 @@
     <t xml:space="preserve">37.22% (0.21%) </t>
   </si>
   <si>
-    <t>0.09 [0.09, 0.09]</t>
+    <t xml:space="preserve">0.09 [0.09, 0.09]</t>
   </si>
   <si>
     <t xml:space="preserve">22.10% (0.24%) </t>
@@ -295,10 +287,10 @@
     <t xml:space="preserve">37.28% (0.31%) </t>
   </si>
   <si>
-    <t>.994 [.993, .994]</t>
-  </si>
-  <si>
-    <t>NPV</t>
+    <t xml:space="preserve">.994 [.993, .994]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NPV</t>
   </si>
   <si>
     <t xml:space="preserve">98.96% (0.01%) </t>
@@ -307,7 +299,7 @@
     <t xml:space="preserve">98.93% (0.01%) </t>
   </si>
   <si>
-    <t>-0.00 [-0.00, -0.00]</t>
+    <t xml:space="preserve">-0.00 [-0.00, -0.00]</t>
   </si>
   <si>
     <t xml:space="preserve">99.43% (0.01%) </t>
@@ -331,296 +323,251 @@
     <t xml:space="preserve">98.73% (0.02%) </t>
   </si>
   <si>
-    <t>.979 [.978, .982]</t>
-  </si>
-  <si>
-    <t>Anxiety</t>
-  </si>
-  <si>
-    <t>6.94 (0.11)</t>
-  </si>
-  <si>
-    <t>7.40 (0.12)</t>
-  </si>
-  <si>
-    <t>0.46 [0.45, 0.47]</t>
-  </si>
-  <si>
-    <t>6.05 (0.11)</t>
-  </si>
-  <si>
-    <t>7.18 (0.11)</t>
-  </si>
-  <si>
-    <t>6.20 (0.11)</t>
-  </si>
-  <si>
-    <t>.952 [.950, .954]</t>
-  </si>
-  <si>
-    <t>7.17 (0.11)</t>
-  </si>
-  <si>
-    <t>4.58 (0.11)</t>
-  </si>
-  <si>
-    <t>5.67 (0.12)</t>
-  </si>
-  <si>
-    <t>5.96 (0.11)</t>
-  </si>
-  <si>
-    <t>.985 [.984, .987]</t>
-  </si>
-  <si>
-    <t>Perceived Stress</t>
-  </si>
-  <si>
-    <t>2.90 (0.10)</t>
-  </si>
-  <si>
-    <t>4.34 (0.11)</t>
-  </si>
-  <si>
-    <t>1.44 [1.44, 1.45]</t>
-  </si>
-  <si>
-    <t>2.26 (0.10)</t>
-  </si>
-  <si>
-    <t>3.67 (0.11)</t>
-  </si>
-  <si>
-    <t>.988 [.987, .989]</t>
-  </si>
-  <si>
-    <t>3.48 (0.10)</t>
-  </si>
-  <si>
-    <t>2.31 (0.10)</t>
-  </si>
-  <si>
-    <t>3.29 (0.11)</t>
-  </si>
-  <si>
-    <t>3.43 (0.11)</t>
-  </si>
-  <si>
-    <t>.956 [.954, .961]</t>
-  </si>
-  <si>
-    <t>Academic Burn-out</t>
-  </si>
-  <si>
-    <t>2.65 (0.11)</t>
-  </si>
-  <si>
-    <t>2.82 (0.11)</t>
-  </si>
-  <si>
-    <t>0.17 [0.16, 0.18]</t>
-  </si>
-  <si>
-    <t>1.91 (0.11)</t>
-  </si>
-  <si>
-    <t>2.71 (0.11)</t>
-  </si>
-  <si>
-    <t>3.53 (0.11)</t>
-  </si>
-  <si>
-    <t>.972 [.971, .976]</t>
-  </si>
-  <si>
-    <t>2.73 (0.11)</t>
-  </si>
-  <si>
-    <t>1.86 (0.11)</t>
-  </si>
-  <si>
-    <t>2.70 (0.12)</t>
-  </si>
-  <si>
-    <t>2.66 (0.12)</t>
-  </si>
-  <si>
-    <t>.907 [.903, .919]</t>
-  </si>
-  <si>
-    <t>Internet Addiction</t>
-  </si>
-  <si>
-    <t>2.23 (0.09)</t>
-  </si>
-  <si>
-    <t>1.89 (0.09)</t>
-  </si>
-  <si>
-    <t>-0.34 [-0.35, -0.33]</t>
-  </si>
-  <si>
-    <t>2.12 (0.12)</t>
-  </si>
-  <si>
-    <t>2.06 (0.09)</t>
-  </si>
-  <si>
-    <t>1.85 (0.10)</t>
-  </si>
-  <si>
-    <t>.558 [.541, .575]</t>
-  </si>
-  <si>
-    <t>2.05 (0.09)</t>
-  </si>
-  <si>
-    <t>1.84 (0.12)</t>
-  </si>
-  <si>
-    <t>2.06 (0.11)</t>
-  </si>
-  <si>
-    <t>2.00 (0.11)</t>
-  </si>
-  <si>
-    <t>.398 [.380, .415]</t>
-  </si>
-  <si>
-    <t>Non-suicidal Self-injury</t>
-  </si>
-  <si>
-    <t>1.08 (0.15)</t>
-  </si>
-  <si>
-    <t>1.65 (0.16)</t>
-  </si>
-  <si>
-    <t>0.58 [0.57, 0.59]</t>
-  </si>
-  <si>
-    <t>1.15 (0.16)</t>
-  </si>
-  <si>
-    <t>1.52 (0.15)</t>
-  </si>
-  <si>
-    <t>1.42 (0.16)</t>
-  </si>
-  <si>
-    <t>.492 [.473, .510]</t>
-  </si>
-  <si>
-    <t>1.45 (0.17)</t>
-  </si>
-  <si>
-    <t>1.25 (0.13)</t>
-  </si>
-  <si>
-    <t>1.28 (0.16)</t>
-  </si>
-  <si>
-    <t>1.45 (0.16)</t>
-  </si>
-  <si>
-    <t>.265 [.246, .283]</t>
-  </si>
-  <si>
-    <t>Be Bullied</t>
-  </si>
-  <si>
-    <t>0.44 (0.04)</t>
-  </si>
-  <si>
-    <t>0.40 (0.04)</t>
-  </si>
-  <si>
-    <t>-0.04 [-0.05, -0.04]</t>
-  </si>
-  <si>
-    <t>0.55 (0.05)</t>
-  </si>
-  <si>
-    <t>0.37 (0.04)</t>
-  </si>
-  <si>
-    <t>0.47 (0.05)</t>
-  </si>
-  <si>
-    <t>.683 [.670, .695]</t>
-  </si>
-  <si>
-    <t>0.45 (0.04)</t>
-  </si>
-  <si>
-    <t>0.43 (0.08)</t>
-  </si>
-  <si>
-    <t>0.37 (0.06)</t>
-  </si>
-  <si>
-    <t>0.51 (0.05)</t>
-  </si>
-  <si>
-    <t>.436 [.418, .453]</t>
-  </si>
-  <si>
-    <t>Education Level (Grade)</t>
-  </si>
-  <si>
-    <t>0.45 (0.07)</t>
-  </si>
-  <si>
-    <t>0.19 (0.07)</t>
-  </si>
-  <si>
-    <t>-0.26 [-0.26, -0.25]</t>
-  </si>
-  <si>
-    <t>0.67 (0.13)</t>
-  </si>
-  <si>
-    <t>0.21 (0.13)</t>
-  </si>
-  <si>
-    <t>0.20 (0.12)</t>
-  </si>
-  <si>
-    <t>.744 [.733, .780]</t>
-  </si>
-  <si>
-    <t>0.27 (0.07)</t>
-  </si>
-  <si>
-    <t>0.62 (0.10)</t>
-  </si>
-  <si>
-    <t>0.38 (0.08)</t>
-  </si>
-  <si>
-    <t>0.42 (0.08)</t>
-  </si>
-  <si>
-    <t>.694 [.683, .705]</t>
+    <t xml:space="preserve">.979 [.978, .982]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anxiety</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.94 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.40 (0.12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.46 [0.45, 0.47]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.05 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.18 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.20 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.952 [.950, .954]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.17 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.58 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.67 (0.12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.96 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.985 [.984, .987]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perceived Stress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.90 (0.10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.34 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.44 [1.44, 1.45]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.26 (0.10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.67 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.988 [.987, .989]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.48 (0.10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.31 (0.10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.29 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.43 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.956 [.954, .961]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Academic Burn-out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.65 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.82 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.17 [0.16, 0.18]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.91 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.71 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.53 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.972 [.971, .976]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.73 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.86 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.70 (0.12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.66 (0.12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.907 [.903, .919]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internet Addiction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.23 (0.09)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.89 (0.09)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.34 [-0.35, -0.33]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.12 (0.12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.06 (0.09)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.85 (0.10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.558 [.541, .575]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.05 (0.09)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.84 (0.12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.06 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.00 (0.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.398 [.380, .415]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-suicidal Self-injury</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.08 (0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.65 (0.16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.58 [0.57, 0.59]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.15 (0.16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.52 (0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.42 (0.16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.492 [.473, .510]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.45 (0.17)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.25 (0.13)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.28 (0.16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.45 (0.16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.265 [.246, .283]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Be Bullied</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.44 (0.04)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.40 (0.04)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.04 [-0.05, -0.04]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.55 (0.05)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.37 (0.04)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.47 (0.05)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.683 [.670, .695]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.45 (0.04)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.43 (0.08)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.37 (0.06)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.51 (0.05)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.436 [.418, .453]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -648,18 +595,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -941,28 +879,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="26.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1012,7 +936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1062,7 +986,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1112,7 +1036,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1162,7 +1086,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1212,7 +1136,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -1262,7 +1186,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" t="s">
         <v>80</v>
       </c>
@@ -1312,7 +1236,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" t="s">
         <v>92</v>
       </c>
@@ -1362,7 +1286,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" t="s">
         <v>104</v>
       </c>
@@ -1412,7 +1336,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -1462,7 +1386,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" t="s">
         <v>129</v>
       </c>
@@ -1512,7 +1436,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" t="s">
         <v>142</v>
       </c>
@@ -1562,7 +1486,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" t="s">
         <v>155</v>
       </c>
@@ -1612,7 +1536,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" t="s">
         <v>168</v>
       </c>
@@ -1662,59 +1586,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>181</v>
-      </c>
-      <c r="B15" t="s">
-        <v>182</v>
-      </c>
-      <c r="C15" t="s">
-        <v>183</v>
-      </c>
-      <c r="D15" t="s">
-        <v>184</v>
-      </c>
-      <c r="E15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" t="s">
-        <v>185</v>
-      </c>
-      <c r="G15" t="s">
-        <v>186</v>
-      </c>
-      <c r="H15" t="s">
-        <v>187</v>
-      </c>
-      <c r="I15" t="s">
-        <v>188</v>
-      </c>
-      <c r="J15" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" t="s">
-        <v>189</v>
-      </c>
-      <c r="L15" t="s">
-        <v>190</v>
-      </c>
-      <c r="M15" t="s">
-        <v>191</v>
-      </c>
-      <c r="N15" t="s">
-        <v>192</v>
-      </c>
-      <c r="O15" t="s">
-        <v>193</v>
-      </c>
-      <c r="P15" t="s">
-        <v>20</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>